<commit_message>
Added the conditions for when theres no data
</commit_message>
<xml_diff>
--- a/RPAAirAndOceanCarrierStatuses.xlsx
+++ b/RPAAirAndOceanCarrierStatuses.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\OneDrive - Blume Global\UiPath\OceanCarrierRPA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\blume-proj\OceanCarrierRPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2641,7 +2641,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2760,11 +2760,11 @@
       </c>
       <c r="J5">
         <f>COUNTIF(E4:E45, "done")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K5">
         <f>COUNTIF(E4:E45,"in progress")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <f>COUNTIF(E4:E45,"*blocked*")</f>
@@ -2977,7 +2977,7 @@
       </c>
       <c r="C22" s="2"/>
       <c r="E22" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
another update to status
</commit_message>
<xml_diff>
--- a/RPAAirAndOceanCarrierStatuses.xlsx
+++ b/RPAAirAndOceanCarrierStatuses.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\Dropbox (Blume Global)\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\OneDrive - Blume Global\UiPath\OceanCarrierRPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="180">
   <si>
     <t>V-00181--ITG TRANSPORTATION SERVICES INC</t>
   </si>
@@ -2656,7 +2656,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2878,7 +2878,9 @@
       <c r="B9" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>178</v>
+      </c>
       <c r="E9" t="s">
         <v>155</v>
       </c>
@@ -3084,7 +3086,7 @@
         <v>117</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="E25" t="s">
         <v>155</v>
@@ -3158,7 +3160,9 @@
       <c r="B30" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="C30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>178</v>
+      </c>
       <c r="E30" t="s">
         <v>155</v>
       </c>
@@ -3185,7 +3189,9 @@
       <c r="B32" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="C32" s="2"/>
+      <c r="C32" s="2" t="s">
+        <v>178</v>
+      </c>
       <c r="E32" t="s">
         <v>174</v>
       </c>
@@ -3329,7 +3335,9 @@
       <c r="B44" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="C44" s="2"/>
+      <c r="C44" s="2" t="s">
+        <v>178</v>
+      </c>
       <c r="E44" t="s">
         <v>155</v>
       </c>

</xml_diff>